<commit_message>
API-14 Create new page for import students list
- A whole new page only for import Student
- Upload file button added
- Reset button so that the uploaded file can be deleted
- 'Import Student' button to started import students into Student table
- A big Error Box for displaying specific error message of the fields located in the Excel file
</commit_message>
<xml_diff>
--- a/server/data/students.xlsx
+++ b/server/data/students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Projects\newhope-baito\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5904DA8F-7953-4385-831B-1A42FADDB6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1749EAEF-E630-439E-AEC8-A6478389F757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31605" yWindow="2790" windowWidth="17250" windowHeight="8865" xr2:uid="{2AD62F3D-8F82-43A9-91C1-2E4D282AE558}"/>
+    <workbookView xWindow="31905" yWindow="2400" windowWidth="21600" windowHeight="11235" xr2:uid="{2AD62F3D-8F82-43A9-91C1-2E4D282AE558}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Full Name</t>
   </si>
@@ -99,16 +99,39 @@
   </si>
   <si>
     <t>German</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>liam.nguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>emma.tran@gmail.com</t>
+  </si>
+  <si>
+    <t>15/05/200</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,15 +154,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,121 +498,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779A31DE-2644-46CD-90E3-FAA5CFE37FFA}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
-        <v>37756</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1">
         <v>38311</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="D10" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{0ECBB394-F232-4DA5-BF25-8C99E9BDE8AF}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{277E2E74-8A70-4F3E-8DF3-09B2C11D2758}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>